<commit_message>
Ke Hoach An Toan
</commit_message>
<xml_diff>
--- a/TongHopDuThau.xlsx
+++ b/TongHopDuThau.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8300627D-CFAF-4802-A901-26E52BF6D45E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="768" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="768" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TBMT" sheetId="2" r:id="rId1"/>
@@ -44,7 +45,7 @@
     <definedName name="tbmt">TBMT!$A:$J</definedName>
     <definedName name="TT">[3]DG!$A$5:$I$1419</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="746">
   <si>
     <t>CongTrinh</t>
   </si>
@@ -2346,11 +2347,14 @@
   <si>
     <t>01/09/2020</t>
   </si>
+  <si>
+    <t>Xây dựng mới đường dây hạ thế để xử lý các dây Brancherment băng đường huyện Xuân Lộc năm 2018</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="dd/mm"/>
@@ -3044,11 +3048,11 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="5"/>
+    <cellStyle name="Comma 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="40">
     <dxf>
@@ -3489,7 +3493,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0F89E8A-03A1-4553-82C9-870FBDF5B443}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0F89E8A-03A1-4553-82C9-870FBDF5B443}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -63802,7 +63806,7 @@
       <definedName name="VND"/>
     </definedNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -64063,31 +64067,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:M41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="103" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="42.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" style="103" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="103" t="str">
         <f>LEFT(D1,11)</f>
         <v/>
@@ -64107,7 +64111,7 @@
       <c r="L1" s="41"/>
       <c r="M1" s="41"/>
     </row>
-    <row r="2" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="104" t="str">
         <f>TRIM(B2)</f>
         <v/>
@@ -64125,7 +64129,7 @@
       <c r="L2" s="41"/>
       <c r="M2" s="41"/>
     </row>
-    <row r="3" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="104" t="str">
         <f t="shared" ref="A3:A39" si="0">TRIM(B3)</f>
         <v/>
@@ -64143,7 +64147,7 @@
       <c r="L3" s="41"/>
       <c r="M3" s="41"/>
     </row>
-    <row r="4" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -64161,7 +64165,7 @@
       <c r="L4" s="41"/>
       <c r="M4" s="41"/>
     </row>
-    <row r="5" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="104" t="str">
         <f>TRIM(B5)</f>
         <v/>
@@ -64179,7 +64183,7 @@
       <c r="L5" s="41"/>
       <c r="M5" s="41"/>
     </row>
-    <row r="6" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -64197,7 +64201,7 @@
       <c r="L6" s="41"/>
       <c r="M6" s="41"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Thông tin chung</v>
@@ -64217,7 +64221,7 @@
       <c r="L7" s="41"/>
       <c r="M7" s="41"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Số TBMT</v>
@@ -64243,7 +64247,7 @@
       <c r="L8" s="41"/>
       <c r="M8" s="41"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Hình thức thông báo</v>
@@ -64265,7 +64269,7 @@
       <c r="L9" s="41"/>
       <c r="M9" s="41"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Loại thông báo</v>
@@ -64291,7 +64295,7 @@
       <c r="L10" s="41"/>
       <c r="M10" s="41"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Bên mời thầu</v>
@@ -64313,7 +64317,7 @@
       <c r="L11" s="41"/>
       <c r="M11" s="41"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Chủ đầu tư</v>
@@ -64335,7 +64339,7 @@
       <c r="L12" s="41"/>
       <c r="M12" s="41"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Phân loại</v>
@@ -64357,7 +64361,7 @@
       <c r="L13" s="41"/>
       <c r="M13" s="41"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Tên gói thầu</v>
@@ -64379,7 +64383,7 @@
       <c r="L14" s="41"/>
       <c r="M14" s="41"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Tên dự án</v>
@@ -64401,7 +64405,7 @@
       <c r="L15" s="41"/>
       <c r="M15" s="41"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Nguồn vốn</v>
@@ -64423,7 +64427,7 @@
       <c r="L16" s="41"/>
       <c r="M16" s="41"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Phương thức</v>
@@ -64445,7 +64449,7 @@
       <c r="L17" s="41"/>
       <c r="M17" s="41"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Thời gian thực hiện hợp đồng</v>
@@ -64467,7 +64471,7 @@
       <c r="L18" s="41"/>
       <c r="M18" s="41"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Nội dung chính gói thầu</v>
@@ -64487,7 +64491,7 @@
       <c r="L19" s="41"/>
       <c r="M19" s="41"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Loại hợp đồng</v>
@@ -64509,7 +64513,7 @@
       <c r="L20" s="41"/>
       <c r="M20" s="41"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Hình thức đấu thầu</v>
@@ -64533,7 +64537,7 @@
       <c r="L21" s="41"/>
       <c r="M21" s="41"/>
     </row>
-    <row r="22" spans="1:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -64551,7 +64555,7 @@
       <c r="L22" s="41"/>
       <c r="M22" s="41"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Tham dự thầu</v>
@@ -64571,7 +64575,7 @@
       <c r="L23" s="41"/>
       <c r="M23" s="41"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Hình thức nhận HSDT</v>
@@ -64593,7 +64597,7 @@
       <c r="L24" s="41"/>
       <c r="M24" s="41"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Thời gian nhận HSDT từ ngày</v>
@@ -64619,7 +64623,7 @@
       <c r="L25" s="41"/>
       <c r="M25" s="41"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Mua HSMT</v>
@@ -64641,7 +64645,7 @@
       <c r="L26" s="41"/>
       <c r="M26" s="41"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Địa điểm nhận HSDT</v>
@@ -64663,7 +64667,7 @@
       <c r="L27" s="41"/>
       <c r="M27" s="41"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -64681,7 +64685,7 @@
       <c r="L28" s="41"/>
       <c r="M28" s="41"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Mở thầu</v>
@@ -64701,7 +64705,7 @@
       <c r="L29" s="41"/>
       <c r="M29" s="41"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Thời điểm mở thầu</v>
@@ -64723,7 +64727,7 @@
       <c r="L30" s="41"/>
       <c r="M30" s="41"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Địa điểm mở thầu</v>
@@ -64745,7 +64749,7 @@
       <c r="L31" s="41"/>
       <c r="M31" s="41"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Giá gói thầu</v>
@@ -64767,7 +64771,7 @@
       <c r="L32" s="41"/>
       <c r="M32" s="41"/>
     </row>
-    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Số tiền bằng chữ</v>
@@ -64781,7 +64785,7 @@
       </c>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -64791,7 +64795,7 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Bảo đảm dự thầu</v>
@@ -64803,7 +64807,7 @@
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Hình thức đảm bảo</v>
@@ -64817,7 +64821,7 @@
       </c>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Số tiền đảm bảo</v>
@@ -64831,7 +64835,7 @@
       </c>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="104" t="str">
         <f t="shared" si="0"/>
         <v>Số tiền bằng chữ</v>
@@ -64845,7 +64849,7 @@
       </c>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -64862,22 +64866,22 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B1:J16"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="58.7109375" style="41" customWidth="1"/>
-    <col min="5" max="9" width="32.42578125" style="94" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="58.6640625" style="41" customWidth="1"/>
+    <col min="5" max="9" width="32.44140625" style="94" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="45" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" s="45" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="95" t="s">
         <v>102</v>
       </c>
@@ -64906,7 +64910,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="93.6" x14ac:dyDescent="0.3">
       <c r="B2" s="96">
         <v>1</v>
       </c>
@@ -64927,7 +64931,7 @@
       <c r="I2" s="120"/>
       <c r="J2" s="120"/>
     </row>
-    <row r="3" spans="2:10" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="93.6" x14ac:dyDescent="0.3">
       <c r="B3" s="96">
         <v>2</v>
       </c>
@@ -64948,7 +64952,7 @@
       <c r="I3" s="120"/>
       <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="2:10" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="78" x14ac:dyDescent="0.3">
       <c r="B4" s="96">
         <v>3</v>
       </c>
@@ -64969,7 +64973,7 @@
       <c r="I4" s="121"/>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="96">
         <v>4</v>
       </c>
@@ -64991,7 +64995,7 @@
       <c r="I5" s="121"/>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="96">
         <v>5</v>
       </c>
@@ -65013,7 +65017,7 @@
       <c r="I6" s="121"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B7" s="96">
         <v>6</v>
       </c>
@@ -65034,7 +65038,7 @@
       <c r="I7" s="120"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B8" s="96">
         <v>7</v>
       </c>
@@ -65055,7 +65059,7 @@
       <c r="I8" s="121"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B9" s="96">
         <v>8</v>
       </c>
@@ -65074,7 +65078,7 @@
       <c r="I9" s="121"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B10" s="96">
         <v>9</v>
       </c>
@@ -65093,7 +65097,7 @@
       <c r="I10" s="121"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B11" s="96">
         <v>10</v>
       </c>
@@ -65112,7 +65116,7 @@
       <c r="I11" s="121"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B12" s="96">
         <v>11</v>
       </c>
@@ -65137,7 +65141,7 @@
       <c r="I12" s="120"/>
       <c r="J12" s="120"/>
     </row>
-    <row r="13" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B13" s="96">
         <v>12</v>
       </c>
@@ -65158,7 +65162,7 @@
       <c r="I13" s="121"/>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B14" s="96">
         <v>13</v>
       </c>
@@ -65180,7 +65184,7 @@
       <c r="I14" s="124"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B15" s="96">
         <v>14</v>
       </c>
@@ -65199,7 +65203,7 @@
       <c r="I15" s="124"/>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="2:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B16" s="96">
         <v>15</v>
       </c>
@@ -65219,7 +65223,7 @@
       <c r="J16" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:J16"/>
+  <autoFilter ref="B1:J16" xr:uid="{00000000-0009-0000-0000-000009000000}"/>
   <conditionalFormatting sqref="E13:I1048576 E12:G12 I12 E2:I11">
     <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThan">
       <formula>0</formula>
@@ -65236,7 +65240,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -65249,26 +65253,26 @@
       <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="72" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" style="72" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" style="72" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" customWidth="1"/>
+    <col min="16" max="16" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="92" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="92" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="92" t="s">
         <v>125</v>
       </c>
@@ -65318,7 +65322,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>696</v>
       </c>
@@ -65341,7 +65345,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>696</v>
       </c>
@@ -65364,7 +65368,7 @@
         <v>44562</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>696</v>
       </c>
@@ -65387,7 +65391,7 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>696</v>
       </c>
@@ -65410,7 +65414,7 @@
         <v>47107</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>696</v>
       </c>
@@ -65430,7 +65434,7 @@
         <v>1900000000</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>696</v>
       </c>
@@ -65447,7 +65451,7 @@
         <v>44196</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>696</v>
       </c>
@@ -65473,7 +65477,7 @@
         <v>44139</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>696</v>
       </c>
@@ -65496,7 +65500,7 @@
         <v>44145</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>715</v>
       </c>
@@ -65531,7 +65535,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>715</v>
       </c>
@@ -65569,7 +65573,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>715</v>
       </c>
@@ -65604,7 +65608,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>715</v>
       </c>
@@ -65643,7 +65647,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>715</v>
       </c>
@@ -65681,7 +65685,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>715</v>
       </c>
@@ -65722,7 +65726,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>727</v>
       </c>
@@ -65739,7 +65743,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>727</v>
       </c>
@@ -65756,7 +65760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>727</v>
       </c>
@@ -65773,7 +65777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>727</v>
       </c>
@@ -65790,7 +65794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>727</v>
       </c>
@@ -65807,7 +65811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>727</v>
       </c>
@@ -65824,7 +65828,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>727</v>
       </c>
@@ -65841,7 +65845,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>727</v>
       </c>
@@ -65859,7 +65863,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J4"/>
+  <autoFilter ref="A1:J4" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>
   <conditionalFormatting sqref="H1:I7 H9:I10 H16:I17 H19:I1048576">
     <cfRule type="cellIs" dxfId="14" priority="10" operator="between">
       <formula>1</formula>
@@ -65897,19 +65901,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:I14">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="between">
       <formula>1</formula>
       <formula>TODAY()+30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
       <formula>1</formula>
       <formula>TODAY()+30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:I18">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="between">
       <formula>1</formula>
       <formula>TODAY()+30</formula>
     </cfRule>
@@ -65920,7 +65924,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:W79"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -65929,27 +65933,27 @@
       <selection pane="bottomLeft" activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="24"/>
+    <col min="1" max="1" width="16.44140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="24"/>
     <col min="3" max="3" width="13" style="24" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="27"/>
-    <col min="5" max="5" width="8.85546875" style="24"/>
-    <col min="6" max="6" width="30.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.5703125" style="24" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" style="24" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="25" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="24"/>
+    <col min="4" max="4" width="8.88671875" style="27"/>
+    <col min="5" max="5" width="8.88671875" style="24"/>
+    <col min="6" max="6" width="30.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.5546875" style="24" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="24" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" style="25" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="24"/>
     <col min="13" max="13" width="13" style="27" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" style="27" customWidth="1"/>
-    <col min="15" max="15" width="50.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" style="24" customWidth="1"/>
-    <col min="17" max="16384" width="8.85546875" style="24"/>
+    <col min="14" max="14" width="16.109375" style="27" customWidth="1"/>
+    <col min="15" max="15" width="50.5546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" style="24" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>552</v>
       </c>
@@ -66001,7 +66005,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="55" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -66058,7 +66062,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>107</v>
       </c>
@@ -66099,7 +66103,7 @@
         <v>29696</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="55" t="s">
         <v>468</v>
       </c>
@@ -66139,7 +66143,7 @@
         <v>40360</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>107</v>
       </c>
@@ -66180,7 +66184,7 @@
         <v>36242</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>107</v>
       </c>
@@ -66221,7 +66225,7 @@
         <v>34970</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B7" s="55"/>
       <c r="D7" s="27">
         <f>COUNTIF($B$1:B7,"x")</f>
@@ -66256,7 +66260,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B8" s="55"/>
       <c r="D8" s="27">
         <f>COUNTIF($B$1:B8,"x")</f>
@@ -66294,7 +66298,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>107</v>
       </c>
@@ -66335,7 +66339,7 @@
         <v>33816</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="D10" s="27">
         <f>COUNTIF($B$1:B10,"x")</f>
         <v>4</v>
@@ -66356,7 +66360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B11" s="55"/>
       <c r="D11" s="27">
         <f>COUNTIF($B$1:B11,"x")</f>
@@ -66391,7 +66395,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>107</v>
       </c>
@@ -66432,7 +66436,7 @@
         <v>35580</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="D13" s="27">
         <f>COUNTIF($B$1:B13,"x")</f>
         <v>5</v>
@@ -66457,7 +66461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="D14" s="27">
         <f>COUNTIF($B$1:B14,"x")</f>
         <v>5</v>
@@ -66482,7 +66486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>107</v>
       </c>
@@ -66523,7 +66527,7 @@
         <v>27567</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>107</v>
       </c>
@@ -66564,7 +66568,7 @@
         <v>36767</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>107</v>
       </c>
@@ -66605,7 +66609,7 @@
         <v>36804</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
         <v>107</v>
       </c>
@@ -66646,7 +66650,7 @@
         <v>29205</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D19" s="27">
         <f>COUNTIF($B$1:B19,"x")</f>
         <v>9</v>
@@ -66671,7 +66675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D20" s="27">
         <f>COUNTIF($B$1:B20,"x")</f>
         <v>9</v>
@@ -66696,7 +66700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D21" s="27">
         <f>COUNTIF($B$1:B21,"x")</f>
         <v>9</v>
@@ -66724,7 +66728,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>107</v>
       </c>
@@ -66765,7 +66769,7 @@
         <v>35884</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>107</v>
       </c>
@@ -66806,7 +66810,7 @@
         <v>31088</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D24" s="27">
         <f>COUNTIF($B$1:B24,"x")</f>
         <v>11</v>
@@ -66831,7 +66835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>107</v>
       </c>
@@ -66872,7 +66876,7 @@
         <v>37008</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>107</v>
       </c>
@@ -66913,7 +66917,7 @@
         <v>31416</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B27" s="55"/>
       <c r="D27" s="27">
         <f>COUNTIF($B$1:B27,"x")</f>
@@ -66948,7 +66952,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D28" s="27">
         <f>COUNTIF($B$1:B28,"x")</f>
         <v>13</v>
@@ -66969,7 +66973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B29" s="55"/>
       <c r="D29" s="27">
         <f>COUNTIF($B$1:B29,"x")</f>
@@ -67004,7 +67008,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D30" s="27">
         <f>COUNTIF($B$1:B30,"x")</f>
         <v>13</v>
@@ -67025,7 +67029,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
         <v>107</v>
       </c>
@@ -67066,7 +67070,7 @@
         <v>34041</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D32" s="27">
         <f>COUNTIF($B$1:B32,"x")</f>
         <v>14</v>
@@ -67091,7 +67095,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>107</v>
       </c>
@@ -67132,7 +67136,7 @@
         <v>35555</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B34" s="55"/>
       <c r="D34" s="27">
         <f>COUNTIF($B$1:B34,"x")</f>
@@ -67164,7 +67168,7 @@
         <v>29587</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="24" t="s">
         <v>107</v>
       </c>
@@ -67205,7 +67209,7 @@
         <v>34976</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B36" s="55"/>
       <c r="D36" s="27">
         <f>COUNTIF($B$1:B36,"x")</f>
@@ -67240,7 +67244,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B37" s="55"/>
       <c r="D37" s="27">
         <f>COUNTIF($B$1:B37,"x")</f>
@@ -67275,7 +67279,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B38" s="55"/>
       <c r="D38" s="27">
         <f>COUNTIF($B$1:B38,"x")</f>
@@ -67310,7 +67314,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="24" t="s">
         <v>107</v>
       </c>
@@ -67351,7 +67355,7 @@
         <v>29221</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="24" t="s">
         <v>107</v>
       </c>
@@ -67392,7 +67396,7 @@
         <v>30027</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D41" s="27">
         <f>COUNTIF($B$1:B41,"x")</f>
         <v>18</v>
@@ -67417,7 +67421,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="24" t="s">
         <v>107</v>
       </c>
@@ -67453,7 +67457,7 @@
         <v>43103</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B43" s="55"/>
       <c r="D43" s="27">
         <f>COUNTIF($B$1:B43,"x")</f>
@@ -67488,7 +67492,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="24" t="s">
         <v>107</v>
       </c>
@@ -67529,7 +67533,7 @@
         <v>34974</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="24" t="s">
         <v>107</v>
       </c>
@@ -67566,7 +67570,7 @@
         <v>30730</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B46" s="55"/>
       <c r="D46" s="27">
         <f>COUNTIF($B$1:B46,"x")</f>
@@ -67601,7 +67605,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D47" s="27">
         <f>COUNTIF($B$1:B47,"x")</f>
         <v>19</v>
@@ -67626,7 +67630,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D48" s="27">
         <f>COUNTIF($B$1:B48,"x")</f>
         <v>19</v>
@@ -67651,7 +67655,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="24" t="s">
         <v>107</v>
       </c>
@@ -67692,7 +67696,7 @@
         <v>34281</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="24" t="s">
         <v>468</v>
       </c>
@@ -67722,7 +67726,7 @@
         <v>33442</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="24" t="s">
         <v>107</v>
       </c>
@@ -67753,7 +67757,7 @@
         <v>27534</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="24" t="s">
         <v>569</v>
       </c>
@@ -67776,7 +67780,7 @@
         <v>29541</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="24" t="s">
         <v>468</v>
       </c>
@@ -67813,7 +67817,7 @@
         <v>41396</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="24" t="s">
         <v>107</v>
       </c>
@@ -67844,119 +67848,119 @@
         <v>30596</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C60" s="24" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C61" s="24" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C62" s="24" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C63" s="24" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C64" s="24" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C65" s="24" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C66" s="24" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C67" s="24" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C68" s="24" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C69" s="24" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C70" s="24" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C71" s="24" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C72" s="24" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C73" s="24" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C74" s="24" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C75" s="24" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C76" s="24" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C77" s="24" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C78" s="24" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C79" s="24" t="s">
         <v>501</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W54"/>
+  <autoFilter ref="A1:W54" xr:uid="{00000000-0009-0000-0000-00000B000000}"/>
   <conditionalFormatting sqref="F7">
-    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:F53">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F55:F1048576 F8:F51 F1:F6">
-    <cfRule type="duplicateValues" dxfId="5" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="17"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -67964,25 +67968,25 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="B1:O10"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" style="60" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" style="60" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="66" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" ht="64.8" x14ac:dyDescent="0.3">
       <c r="B1" s="62" t="s">
         <v>159</v>
       </c>
@@ -68006,7 +68010,7 @@
         <v>3500000000</v>
       </c>
     </row>
-    <row r="2" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="138" t="s">
         <v>204</v>
       </c>
@@ -68028,7 +68032,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="138"/>
       <c r="C3" s="139"/>
       <c r="D3" s="63" t="s">
@@ -68046,7 +68050,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="138"/>
       <c r="C4" s="139"/>
       <c r="D4" s="63" t="s">
@@ -68066,7 +68070,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="66"/>
       <c r="C5" s="66"/>
       <c r="D5" s="67">
@@ -68090,13 +68094,13 @@
         <v>543</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="E6" s="60"/>
       <c r="I6" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>201</v>
       </c>
@@ -68110,7 +68114,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" ht="62.4" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>2017</v>
       </c>
@@ -68145,7 +68149,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" ht="72" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>2018</v>
       </c>
@@ -68180,7 +68184,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>2019</v>
       </c>
@@ -68202,36 +68206,36 @@
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J5" r:id="rId1"/>
-    <hyperlink ref="L9" r:id="rId2"/>
+    <hyperlink ref="J5" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="L9" r:id="rId2" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="88" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" style="88" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="72" customWidth="1"/>
-    <col min="9" max="9" width="45.42578125" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="72" customWidth="1"/>
+    <col min="9" max="9" width="45.44140625" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="58" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="58" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="86">
         <f>SUMIF(A2:A21,"x",F2:F21)</f>
         <v>1740168722</v>
@@ -68264,7 +68268,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -68293,7 +68297,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>346</v>
       </c>
@@ -68319,7 +68323,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>351</v>
       </c>
@@ -68345,7 +68349,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>354</v>
       </c>
@@ -68371,7 +68375,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>341</v>
       </c>
@@ -68397,7 +68401,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>519</v>
       </c>
@@ -68423,50 +68427,50 @@
         <v>345</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I12">
         <v>1640251089</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I13">
         <v>1374255938</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I14">
         <v>3043578216</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I15">
         <v>1133019615</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I16">
         <v>1276052117</v>
       </c>
     </row>
-    <row r="17" spans="4:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="90"/>
     </row>
-    <row r="18" spans="4:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18" s="90"/>
     </row>
-    <row r="19" spans="4:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D19" s="90"/>
     </row>
-    <row r="20" spans="4:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D20" s="90"/>
     </row>
-    <row r="21" spans="4:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D21" s="90"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J21"/>
+  <autoFilter ref="A1:J21" xr:uid="{00000000-0009-0000-0000-00000D000000}"/>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
       <formula>1</formula>
       <formula>"today()-365*3"</formula>
     </cfRule>
@@ -68476,19 +68480,19 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="D1:J42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D1" t="s">
         <v>171</v>
       </c>
@@ -68508,7 +68512,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="2" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D2">
         <f>IFERROR(VLOOKUP(E2,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68529,7 +68533,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D3">
         <f>IFERROR(VLOOKUP(E3,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68550,7 +68554,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D4">
         <f>IFERROR(VLOOKUP(E4,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68571,7 +68575,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D5">
         <f>IFERROR(VLOOKUP(E5,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68592,7 +68596,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D6">
         <f>IFERROR(VLOOKUP(E6,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68613,7 +68617,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D7">
         <f>IFERROR(VLOOKUP(E7,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68634,7 +68638,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D8">
         <f>IFERROR(VLOOKUP(E8,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68655,7 +68659,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D9">
         <f>IFERROR(VLOOKUP(E9,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68676,7 +68680,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D10">
         <f>IFERROR(VLOOKUP(E10,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68697,7 +68701,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D11">
         <f>IFERROR(VLOOKUP(E11,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68718,7 +68722,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D12">
         <f>IFERROR(VLOOKUP(E12,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68736,7 +68740,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D13">
         <f>IFERROR(VLOOKUP(E13,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68757,7 +68761,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D14">
         <f>IFERROR(VLOOKUP(E14,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68778,7 +68782,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D15">
         <f>IFERROR(VLOOKUP(E15,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68799,7 +68803,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D16">
         <f>IFERROR(VLOOKUP(E16,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68820,7 +68824,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D17">
         <f>IFERROR(VLOOKUP(E17,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68841,7 +68845,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D18">
         <f>IFERROR(VLOOKUP(E18,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68862,7 +68866,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D19">
         <f>IFERROR(VLOOKUP(E19,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68883,7 +68887,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D20">
         <f>IFERROR(VLOOKUP(E20,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68904,7 +68908,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D21">
         <f>IFERROR(VLOOKUP(E21,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68925,7 +68929,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D22">
         <f>IFERROR(VLOOKUP(E22,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68949,7 +68953,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D23">
         <f>IFERROR(VLOOKUP(E23,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68973,7 +68977,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D24">
         <f>IFERROR(VLOOKUP(E24,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -68997,7 +69001,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D25">
         <f>IFERROR(VLOOKUP(E25,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69021,7 +69025,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D26">
         <f>IFERROR(VLOOKUP(E26,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69045,7 +69049,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D27">
         <f>IFERROR(VLOOKUP(E27,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69069,7 +69073,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D28">
         <f>IFERROR(VLOOKUP(E28,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69093,7 +69097,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D29">
         <f>IFERROR(VLOOKUP(E29,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69117,7 +69121,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="30" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D30">
         <f>IFERROR(VLOOKUP(E30,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69141,7 +69145,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="31" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D31">
         <f>IFERROR(VLOOKUP(E31,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69165,7 +69169,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="32" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D32">
         <f>IFERROR(VLOOKUP(E32,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69186,7 +69190,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D33">
         <f>IFERROR(VLOOKUP(E33,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69207,7 +69211,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D34">
         <f>IFERROR(VLOOKUP(E34,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69228,7 +69232,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D35">
         <f>IFERROR(VLOOKUP(E35,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69249,7 +69253,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D36">
         <f>IFERROR(VLOOKUP(E36,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69270,7 +69274,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D37">
         <f>IFERROR(VLOOKUP(E37,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69291,7 +69295,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D38">
         <f>IFERROR(VLOOKUP(E38,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69312,7 +69316,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D39">
         <f>IFERROR(VLOOKUP(E39,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69333,7 +69337,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D40">
         <f>IFERROR(VLOOKUP(E40,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69354,7 +69358,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D41">
         <f>IFERROR(VLOOKUP(E41,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69375,7 +69379,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D42">
         <f>IFERROR(VLOOKUP(E42,NhanSu!F:L,6,0),0)</f>
         <v>0</v>
@@ -69398,7 +69402,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -69408,41 +69412,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="50.5703125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="15" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="15"/>
-    <col min="10" max="10" width="10.42578125" style="15" customWidth="1"/>
-    <col min="11" max="12" width="14.28515625" style="15" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" style="15" customWidth="1"/>
-    <col min="14" max="14" width="14" style="70" customWidth="1"/>
-    <col min="15" max="16" width="18.5703125" style="15" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.28515625" style="15" customWidth="1"/>
-    <col min="20" max="20" width="14.7109375" style="15" customWidth="1"/>
-    <col min="21" max="21" width="20.5703125" style="15" customWidth="1"/>
-    <col min="22" max="22" width="25.140625" style="15" customWidth="1"/>
-    <col min="23" max="16384" width="8.85546875" style="15"/>
+    <col min="1" max="1" width="17.44140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="50.5546875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="52.5546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="15" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="19.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="15"/>
+    <col min="10" max="10" width="10.44140625" style="15" customWidth="1"/>
+    <col min="11" max="12" width="14.33203125" style="15" customWidth="1"/>
+    <col min="13" max="13" width="17.88671875" style="15" customWidth="1"/>
+    <col min="14" max="14" width="16" style="70" customWidth="1"/>
+    <col min="15" max="16" width="18.5546875" style="15" customWidth="1"/>
+    <col min="17" max="17" width="14.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.33203125" style="15" customWidth="1"/>
+    <col min="20" max="20" width="14.6640625" style="15" customWidth="1"/>
+    <col min="21" max="21" width="20.5546875" style="15" customWidth="1"/>
+    <col min="22" max="22" width="25.109375" style="15" customWidth="1"/>
+    <col min="23" max="16384" width="8.88671875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
@@ -69555,7 +69559,7 @@
         <v>01/09/2021</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="17" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="17" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>679</v>
       </c>
@@ -69597,7 +69601,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="17" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" s="17" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>20200563645</v>
       </c>
@@ -69640,7 +69644,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>636</v>
       </c>
@@ -69682,7 +69686,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="22" t="s">
         <v>628</v>
       </c>
@@ -69720,7 +69724,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>616</v>
       </c>
@@ -69764,7 +69768,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="22" t="s">
         <v>579</v>
       </c>
@@ -69808,7 +69812,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>570</v>
       </c>
@@ -69852,7 +69856,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>562</v>
       </c>
@@ -69888,7 +69892,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>20191257175</v>
       </c>
@@ -69935,7 +69939,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>96</v>
       </c>
@@ -69981,7 +69985,7 @@
         <v>44201</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>101</v>
       </c>
@@ -70025,7 +70029,7 @@
         <v>44201</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="132" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" s="132" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="129" t="s">
         <v>214</v>
       </c>
@@ -70078,7 +70082,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="17" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" s="17" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>232</v>
       </c>
@@ -70120,7 +70124,7 @@
       </c>
       <c r="N15" s="71"/>
     </row>
-    <row r="16" spans="1:21" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>242</v>
       </c>
@@ -70175,7 +70179,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>253</v>
       </c>
@@ -70213,7 +70217,7 @@
         <v>44273.345138888886</v>
       </c>
     </row>
-    <row r="18" spans="1:20" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>263</v>
       </c>
@@ -70271,12 +70275,12 @@
       <c r="S18" s="17">
         <v>1481983404</v>
       </c>
-      <c r="T18" s="17" t="e">
+      <c r="T18" s="17" t="str">
         <f>[4]!VND(S18)</f>
-        <v>#VALUE!</v>
+        <v>Một tỷ, bốn trăm tám mươi mốt triệu, chín trăm tám mươi ba nghìn, bốn trăm lẻ bốn đồng chẵn.</v>
       </c>
     </row>
-    <row r="19" spans="1:20" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>297</v>
       </c>
@@ -70313,7 +70317,7 @@
         <v>44277</v>
       </c>
     </row>
-    <row r="20" spans="1:20" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
         <v>435</v>
       </c>
@@ -70349,7 +70353,7 @@
         <v>44274.34375</v>
       </c>
     </row>
-    <row r="21" spans="1:20" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>464</v>
       </c>
@@ -70385,7 +70389,7 @@
         <v>44279.334027777775</v>
       </c>
     </row>
-    <row r="22" spans="1:20" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>469</v>
       </c>
@@ -70421,7 +70425,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="23" spans="1:20" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>472</v>
       </c>
@@ -70457,7 +70461,7 @@
         <v>44291</v>
       </c>
     </row>
-    <row r="24" spans="1:20" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
         <v>482</v>
       </c>
@@ -70495,7 +70499,7 @@
         <v>01/09/2021</v>
       </c>
     </row>
-    <row r="25" spans="1:20" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>522</v>
       </c>
@@ -70539,7 +70543,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="26" spans="1:20" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>546</v>
       </c>
@@ -70583,7 +70587,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="27" spans="1:20" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>546</v>
       </c>
@@ -70618,7 +70622,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="28" spans="1:20" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>546</v>
       </c>
@@ -70651,6 +70655,17 @@
       </c>
       <c r="N28" s="49" t="s">
         <v>550</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B29" s="15" t="s">
+        <v>745</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>523</v>
       </c>
     </row>
   </sheetData>
@@ -70706,20 +70721,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="D1:M24"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M18" sqref="M18:M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="42.140625" customWidth="1"/>
+    <col min="4" max="4" width="42.109375" customWidth="1"/>
     <col min="13" max="13" width="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D1">
         <f>COLUMN()-COLUMN($C$1)</f>
         <v>1</v>
@@ -70756,7 +70771,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>380</v>
       </c>
@@ -70786,7 +70801,7 @@
         <v>Tiết diện dây [mm2]: 50/8</v>
       </c>
     </row>
-    <row r="3" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>381</v>
       </c>
@@ -70816,7 +70831,7 @@
         <v>Đường kính ngoài của ruột dẫn đối với dây trần hay bọc [mm] : 9,5-10</v>
       </c>
     </row>
-    <row r="4" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>388</v>
       </c>
@@ -70846,7 +70861,7 @@
         <v>Độ dày lớp bọc cách điện XLPE 22kV : 5,5 mm</v>
       </c>
     </row>
-    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>390</v>
       </c>
@@ -70876,7 +70891,7 @@
         <v>Đường kính ngoài của dây bọc 22kV [mm]: 23,1-23,4</v>
       </c>
     </row>
-    <row r="6" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
         <v>396</v>
       </c>
@@ -70906,7 +70921,7 @@
         <v>Lực kéo đứt [kN]: 17,1</v>
       </c>
     </row>
-    <row r="10" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>380</v>
       </c>
@@ -70921,7 +70936,7 @@
         <v xml:space="preserve">Tiết diện dây [mm2]: </v>
       </c>
     </row>
-    <row r="11" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>410</v>
       </c>
@@ -70936,7 +70951,7 @@
         <v xml:space="preserve">Số tao/đường kính mỗi tao [mm]: </v>
       </c>
     </row>
-    <row r="12" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>413</v>
       </c>
@@ -70951,7 +70966,7 @@
         <v xml:space="preserve">Đường kính ngoài tối đa của cáp [mm]: </v>
       </c>
     </row>
-    <row r="13" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>396</v>
       </c>
@@ -70966,31 +70981,31 @@
         <v xml:space="preserve">Lực kéo đứt [kN]: </v>
       </c>
     </row>
-    <row r="14" spans="4:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:13" x14ac:dyDescent="0.3">
       <c r="M14" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="15" spans="4:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:13" x14ac:dyDescent="0.3">
       <c r="M15" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="16" spans="4:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:13" x14ac:dyDescent="0.3">
       <c r="M16" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="17" spans="4:13" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:13" x14ac:dyDescent="0.3">
       <c r="M17" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">: </v>
       </c>
     </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>380</v>
       </c>
@@ -71017,7 +71032,7 @@
         <v>Tiết diện dây [mm2]: 50/8</v>
       </c>
     </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>381</v>
       </c>
@@ -71044,7 +71059,7 @@
         <v>Đường kính ngoài của ruột dẫn đối với dây trần hay bọc [mm] : 9,5-10</v>
       </c>
     </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>455</v>
       </c>
@@ -71053,7 +71068,7 @@
         <v xml:space="preserve">Độ dày lớp bọc 22kV : </v>
       </c>
     </row>
-    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>456</v>
       </c>
@@ -71083,7 +71098,7 @@
         <v>+ Cách điện XLPE: 5,5 mm</v>
       </c>
     </row>
-    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>457</v>
       </c>
@@ -71113,7 +71128,7 @@
         <v>+ Vỏ ngoài HDPE: 1,2 mm</v>
       </c>
     </row>
-    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>390</v>
       </c>
@@ -71140,7 +71155,7 @@
         <v>Đường kính ngoài của dây bọc 22kV [mm]: 23,1-23,4</v>
       </c>
     </row>
-    <row r="24" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>396</v>
       </c>
@@ -71175,25 +71190,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.85546875" style="109"/>
-    <col min="4" max="4" width="33.85546875" style="110" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="109"/>
+    <col min="1" max="3" width="8.88671875" style="109"/>
+    <col min="4" max="4" width="33.88671875" style="110" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="109"/>
     <col min="6" max="6" width="27" style="109" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="109" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" style="109" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="109"/>
+    <col min="7" max="7" width="7.109375" style="109" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="31.109375" style="109" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="109"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="107" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="107" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="107" t="s">
         <v>125</v>
       </c>
@@ -71219,7 +71234,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D2" s="110" t="s">
         <v>441</v>
       </c>
@@ -71230,7 +71245,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D3" s="110" t="s">
         <v>441</v>
       </c>
@@ -71241,7 +71256,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D4" s="110" t="s">
         <v>441</v>
       </c>
@@ -71253,7 +71268,7 @@
       </c>
       <c r="J4" s="112"/>
     </row>
-    <row r="5" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D5" s="110" t="s">
         <v>440</v>
       </c>
@@ -71265,7 +71280,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D6" s="110" t="s">
         <v>440</v>
       </c>
@@ -71277,7 +71292,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D7" s="110" t="s">
         <v>440</v>
       </c>
@@ -71289,7 +71304,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="110" t="s">
         <v>322</v>
       </c>
@@ -71300,7 +71315,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D9" s="110" t="s">
         <v>322</v>
       </c>
@@ -71311,7 +71326,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D10" s="110" t="s">
         <v>322</v>
       </c>
@@ -71322,7 +71337,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="116" t="s">
         <v>444</v>
       </c>
@@ -71333,7 +71348,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D12" s="116" t="s">
         <v>444</v>
       </c>
@@ -71344,7 +71359,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D13" s="116" t="s">
         <v>444</v>
       </c>
@@ -71355,7 +71370,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="110" t="s">
         <v>445</v>
       </c>
@@ -71366,7 +71381,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D15" s="110" t="s">
         <v>445</v>
       </c>
@@ -71377,7 +71392,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D16" s="110" t="s">
         <v>445</v>
       </c>
@@ -71388,7 +71403,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="17" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D17" s="110" t="s">
         <v>447</v>
       </c>
@@ -71399,7 +71414,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="18" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D18" s="110" t="s">
         <v>447</v>
       </c>
@@ -71410,7 +71425,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="19" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D19" s="110" t="s">
         <v>447</v>
       </c>
@@ -71421,7 +71436,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="20" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D20" s="110" t="s">
         <v>448</v>
       </c>
@@ -71432,7 +71447,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="21" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D21" s="110" t="s">
         <v>448</v>
       </c>
@@ -71443,7 +71458,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="22" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D22" s="110" t="s">
         <v>448</v>
       </c>
@@ -71454,7 +71469,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="23" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D23" s="110" t="s">
         <v>449</v>
       </c>
@@ -71465,7 +71480,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="24" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D24" s="110" t="s">
         <v>452</v>
       </c>
@@ -71476,7 +71491,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="25" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D25" s="110" t="s">
         <v>452</v>
       </c>
@@ -71487,7 +71502,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="26" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D26" s="110" t="s">
         <v>452</v>
       </c>
@@ -71498,7 +71513,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="27" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D27" s="110" t="s">
         <v>460</v>
       </c>
@@ -71509,7 +71524,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="28" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D28" s="110" t="s">
         <v>460</v>
       </c>
@@ -71520,7 +71535,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="29" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D29" s="110" t="s">
         <v>460</v>
       </c>
@@ -71531,7 +71546,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="30" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D30" s="118" t="s">
         <v>461</v>
       </c>
@@ -71542,7 +71557,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="31" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D31" s="118" t="s">
         <v>461</v>
       </c>
@@ -71553,7 +71568,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="32" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D32" s="118" t="s">
         <v>461</v>
       </c>
@@ -71564,7 +71579,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="33" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D33" s="110" t="s">
         <v>256</v>
       </c>
@@ -71575,7 +71590,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="34" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D34" s="110" t="s">
         <v>256</v>
       </c>
@@ -71586,7 +71601,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="35" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D35" s="110" t="s">
         <v>256</v>
       </c>
@@ -71597,7 +71612,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="36" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D36" s="110" t="s">
         <v>534</v>
       </c>
@@ -71608,7 +71623,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D37" s="110" t="s">
         <v>534</v>
       </c>
@@ -71619,7 +71634,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="38" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D38" s="110" t="s">
         <v>534</v>
       </c>
@@ -71630,7 +71645,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="39" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D39" s="110" t="s">
         <v>585</v>
       </c>
@@ -71642,7 +71657,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="40" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D40" s="110" t="s">
         <v>585</v>
       </c>
@@ -71654,7 +71669,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="41" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D41" s="110" t="s">
         <v>585</v>
       </c>
@@ -71666,7 +71681,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="42" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D42" s="110" t="s">
         <v>587</v>
       </c>
@@ -71678,7 +71693,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="43" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D43" s="110" t="s">
         <v>587</v>
       </c>
@@ -71690,7 +71705,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="44" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D44" s="110" t="s">
         <v>587</v>
       </c>
@@ -71702,7 +71717,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="45" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D45" s="110" t="s">
         <v>622</v>
       </c>
@@ -71713,7 +71728,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="46" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D46" s="110" t="s">
         <v>622</v>
       </c>
@@ -71724,7 +71739,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="47" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D47" s="110" t="s">
         <v>622</v>
       </c>
@@ -71735,7 +71750,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="48" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D48" s="110" t="s">
         <v>621</v>
       </c>
@@ -71746,7 +71761,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="49" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D49" s="110" t="s">
         <v>621</v>
       </c>
@@ -71757,7 +71772,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="50" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D50" s="110" t="s">
         <v>621</v>
       </c>
@@ -71766,7 +71781,7 @@
       </c>
       <c r="H50" s="111"/>
     </row>
-    <row r="51" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D51" s="110" t="s">
         <v>621</v>
       </c>
@@ -71777,7 +71792,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="52" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D52" s="110" t="s">
         <v>623</v>
       </c>
@@ -71788,7 +71803,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="53" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D53" s="110" t="s">
         <v>623</v>
       </c>
@@ -71799,7 +71814,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="54" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D54" s="110" t="s">
         <v>623</v>
       </c>
@@ -71808,7 +71823,7 @@
       </c>
       <c r="H54" s="117"/>
     </row>
-    <row r="55" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D55" s="110" t="s">
         <v>623</v>
       </c>
@@ -71819,7 +71834,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="56" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D56" s="110" t="s">
         <v>578</v>
       </c>
@@ -71830,7 +71845,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="57" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
         <v>626</v>
       </c>
@@ -71841,7 +71856,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="58" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D58" s="110" t="s">
         <v>577</v>
       </c>
@@ -71852,7 +71867,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="59" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D59" s="110" t="s">
         <v>646</v>
       </c>
@@ -71863,7 +71878,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="60" spans="4:8" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:8" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D60" s="110" t="s">
         <v>646</v>
       </c>
@@ -71875,18 +71890,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J4"/>
+  <autoFilter ref="A1:J4" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <hyperlinks>
-    <hyperlink ref="H7" r:id="rId1"/>
-    <hyperlink ref="H16" r:id="rId2"/>
-    <hyperlink ref="H19" r:id="rId3"/>
-    <hyperlink ref="H22" r:id="rId4"/>
-    <hyperlink ref="H29" r:id="rId5"/>
-    <hyperlink ref="H32" r:id="rId6"/>
-    <hyperlink ref="H48" r:id="rId7" display="http://lienminhphat.com/"/>
-    <hyperlink ref="H51" r:id="rId8"/>
-    <hyperlink ref="H52" r:id="rId9" display="http://lienminhphat.com/"/>
-    <hyperlink ref="H55" r:id="rId10"/>
+    <hyperlink ref="H7" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="H16" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="H19" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="H22" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="H29" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="H32" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="H48" r:id="rId7" display="http://lienminhphat.com/" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="H51" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="H52" r:id="rId9" display="http://lienminhphat.com/" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="H55" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
@@ -71895,23 +71910,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C1:K38"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="39.28515625" customWidth="1"/>
-    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="39.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.44140625" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
-    <col min="7" max="9" width="8.7109375" style="20" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.6640625" style="20" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:11" s="45" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:11" s="45" customFormat="1" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="46" t="s">
         <v>159</v>
       </c>
@@ -71934,7 +71949,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="38">
         <f>SUM($G$1:G2)</f>
         <v>1</v>
@@ -71958,7 +71973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="38">
         <f>SUM($G$1:G3)</f>
         <v>2</v>
@@ -71982,7 +71997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="38">
         <f>SUM($G$1:G4)</f>
         <v>3</v>
@@ -72009,7 +72024,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="5" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="38">
         <f>SUM($G$1:G5)</f>
         <v>4</v>
@@ -72033,7 +72048,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="6" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="38">
         <f>SUM($G$1:G6)</f>
         <v>5</v>
@@ -72060,7 +72075,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="7" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="38">
         <f>SUM($G$1:G7)</f>
         <v>6</v>
@@ -72084,7 +72099,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="8" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="38">
         <f>SUM($G$1:G8)</f>
         <v>7</v>
@@ -72108,7 +72123,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="9" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="38">
         <f>SUM($G$1:G9)</f>
         <v>8</v>
@@ -72135,7 +72150,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="10" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="38">
         <f>SUM($G$1:G10)</f>
         <v>9</v>
@@ -72162,7 +72177,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="11" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="38">
         <f>SUM($G$1:G11)</f>
         <v>10</v>
@@ -72189,7 +72204,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="12" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="38">
         <f>SUM($G$1:G12)</f>
         <v>11</v>
@@ -72213,7 +72228,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="38">
         <f>SUM($G$1:G13)</f>
         <v>12</v>
@@ -72237,7 +72252,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="14" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="38">
         <f>SUM($G$1:G14)</f>
         <v>13</v>
@@ -72261,7 +72276,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="15" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="38">
         <f>SUM($G$1:G15)</f>
         <v>14</v>
@@ -72285,7 +72300,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="38">
         <f>SUM($G$1:G16)</f>
         <v>15</v>
@@ -72309,7 +72324,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="17" spans="3:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:11" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="38">
         <f>SUM($G$1:G17)</f>
         <v>16</v>
@@ -72333,7 +72348,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="18" spans="3:11" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="38">
         <f>SUM($G$1:G18)</f>
         <v>17</v>
@@ -72357,7 +72372,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="19" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="38">
         <f>SUM($G$1:G19)</f>
         <v>18</v>
@@ -72381,7 +72396,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="20" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="38">
         <f>SUM($G$1:G20)</f>
         <v>19</v>
@@ -72405,7 +72420,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="21" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="38">
         <f>SUM($G$1:G21)</f>
         <v>20</v>
@@ -72429,7 +72444,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="22" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="38">
         <f>SUM($G$1:G22)</f>
         <v>21</v>
@@ -72456,7 +72471,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="23" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="38">
         <f>SUM($G$1:G23)</f>
         <v>22</v>
@@ -72480,7 +72495,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="38">
         <f>SUM($G$1:G24)</f>
         <v>23</v>
@@ -72504,7 +72519,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="25" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="38">
         <f>SUM($G$1:G25)</f>
         <v>24</v>
@@ -72528,7 +72543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="38">
         <f>SUM($G$1:G26)</f>
         <v>25</v>
@@ -72552,7 +72567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="38">
         <f>SUM($G$1:G27)</f>
         <v>26</v>
@@ -72576,7 +72591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="38">
         <f>SUM($G$1:G28)</f>
         <v>27</v>
@@ -72600,7 +72615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="38">
         <f>SUM($G$1:G29)</f>
         <v>28</v>
@@ -72621,7 +72636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="38">
         <f>SUM($G$1:G30)</f>
         <v>29</v>
@@ -72645,7 +72660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C31" s="38">
         <f>SUM($G$1:G31)</f>
         <v>30</v>
@@ -72669,7 +72684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C32" s="38">
         <f>SUM($G$1:G32)</f>
         <v>31</v>
@@ -72693,7 +72708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C33" s="38">
         <f>SUM($G$1:G33)</f>
         <v>32</v>
@@ -72714,7 +72729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="38">
         <f>SUM($G$1:G34)</f>
         <v>33</v>
@@ -72735,7 +72750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="38">
         <f>SUM($G$1:G35)</f>
         <v>34</v>
@@ -72756,7 +72771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" s="38">
         <f>SUM($G$1:G36)</f>
         <v>35</v>
@@ -72780,7 +72795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" s="38">
         <f>SUM($G$1:G37)</f>
         <v>36</v>
@@ -72801,7 +72816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C38" s="38">
         <f>SUM($G$1:G38)</f>
         <v>37</v>
@@ -72823,7 +72838,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:I38"/>
+  <autoFilter ref="C1:I38" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <conditionalFormatting sqref="D11:D1048576 D1:D2 D7 D9">
     <cfRule type="duplicateValues" dxfId="23" priority="7"/>
   </conditionalFormatting>
@@ -72851,30 +72866,30 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="D1:H34"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.85546875" style="7"/>
-    <col min="4" max="4" width="56.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="7"/>
-    <col min="6" max="6" width="40.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="8.88671875" style="7"/>
+    <col min="4" max="4" width="56.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="7"/>
+    <col min="6" max="6" width="40.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="7"/>
+    <col min="9" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D2" s="8" t="s">
         <v>57</v>
       </c>
@@ -72885,7 +72900,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D3" s="9" t="s">
         <v>58</v>
       </c>
@@ -72896,7 +72911,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D4" s="9" t="s">
         <v>59</v>
       </c>
@@ -72907,12 +72922,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D5" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D6" s="9" t="s">
         <v>61</v>
       </c>
@@ -72923,7 +72938,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D7" s="9" t="s">
         <v>62</v>
       </c>
@@ -72937,7 +72952,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D8" s="9" t="s">
         <v>63</v>
       </c>
@@ -72948,7 +72963,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D9" s="9" t="s">
         <v>64</v>
       </c>
@@ -72962,7 +72977,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D10" s="9" t="s">
         <v>65</v>
       </c>
@@ -72976,7 +72991,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D11" s="9" t="s">
         <v>66</v>
       </c>
@@ -72990,7 +73005,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D12" s="9" t="s">
         <v>67</v>
       </c>
@@ -73004,7 +73019,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D13" s="9" t="s">
         <v>68</v>
       </c>
@@ -73018,7 +73033,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D14" s="9" t="s">
         <v>69</v>
       </c>
@@ -73032,7 +73047,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D15" s="9" t="s">
         <v>70</v>
       </c>
@@ -73046,7 +73061,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D16" s="9" t="s">
         <v>71</v>
       </c>
@@ -73060,7 +73075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D17" s="9" t="s">
         <v>72</v>
       </c>
@@ -73074,7 +73089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D18" s="11" t="s">
         <v>57</v>
       </c>
@@ -73088,7 +73103,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D19" s="11" t="s">
         <v>74</v>
       </c>
@@ -73102,7 +73117,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D20" s="11"/>
       <c r="F20" s="3" t="s">
         <v>34</v>
@@ -73114,7 +73129,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D21" s="11" t="s">
         <v>76</v>
       </c>
@@ -73128,7 +73143,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D22" s="11" t="s">
         <v>77</v>
       </c>
@@ -73142,7 +73157,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D23" s="11" t="s">
         <v>78</v>
       </c>
@@ -73156,7 +73171,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D24" s="11" t="s">
         <v>79</v>
       </c>
@@ -73170,7 +73185,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D25" s="11" t="s">
         <v>80</v>
       </c>
@@ -73184,7 +73199,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D26" s="11" t="s">
         <v>75</v>
       </c>
@@ -73198,7 +73213,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D27" s="11" t="s">
         <v>81</v>
       </c>
@@ -73212,7 +73227,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D28" s="11" t="s">
         <v>82</v>
       </c>
@@ -73226,7 +73241,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F29" s="4" t="s">
         <v>47</v>
       </c>
@@ -73237,7 +73252,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F30" s="4" t="s">
         <v>48</v>
       </c>
@@ -73248,7 +73263,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F31" s="3" t="s">
         <v>49</v>
       </c>
@@ -73259,7 +73274,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:8" x14ac:dyDescent="0.3">
       <c r="F32" s="3" t="s">
         <v>51</v>
       </c>
@@ -73270,7 +73285,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F33" s="3" t="s">
         <v>54</v>
       </c>
@@ -73281,7 +73296,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F34" s="3" t="s">
         <v>55</v>
       </c>
@@ -73298,7 +73313,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M47"/>
   <sheetViews>
@@ -73307,20 +73322,20 @@
       <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.85546875" style="84"/>
+    <col min="2" max="2" width="8.88671875" style="84"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="33" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="80" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="80" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="80" t="s">
         <v>125</v>
       </c>
@@ -73361,7 +73376,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>106</v>
       </c>
@@ -73379,7 +73394,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>366</v>
       </c>
@@ -73397,7 +73412,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -73424,7 +73439,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>302</v>
       </c>
@@ -73442,7 +73457,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>125</v>
       </c>
@@ -73469,7 +73484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -73496,7 +73511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>300</v>
       </c>
@@ -73514,7 +73529,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
         <v>486</v>
       </c>
@@ -73527,7 +73542,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>307</v>
       </c>
@@ -73540,7 +73555,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>114</v>
       </c>
@@ -73558,7 +73573,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>113</v>
       </c>
@@ -73576,7 +73591,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>112</v>
       </c>
@@ -73594,7 +73609,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>111</v>
       </c>
@@ -73612,7 +73627,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>110</v>
       </c>
@@ -73630,7 +73645,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>109</v>
       </c>
@@ -73648,7 +73663,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>108</v>
       </c>
@@ -73666,7 +73681,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>106</v>
       </c>
@@ -73684,7 +73699,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>477</v>
       </c>
@@ -73699,7 +73714,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>479</v>
       </c>
@@ -73714,7 +73729,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>480</v>
       </c>
@@ -73729,7 +73744,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>134</v>
       </c>
@@ -73747,7 +73762,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>487</v>
       </c>
@@ -73762,7 +73777,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>127</v>
       </c>
@@ -73780,7 +73795,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>488</v>
       </c>
@@ -73793,7 +73808,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>475</v>
       </c>
@@ -73808,7 +73823,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>150</v>
       </c>
@@ -73823,7 +73838,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>476</v>
       </c>
@@ -73838,7 +73853,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>146</v>
       </c>
@@ -73853,7 +73868,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.45" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>144</v>
       </c>
@@ -73871,7 +73886,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>125</v>
       </c>
@@ -73904,7 +73919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>125</v>
       </c>
@@ -73937,7 +73952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>125</v>
       </c>
@@ -73970,7 +73985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>125</v>
       </c>
@@ -74003,7 +74018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>125</v>
       </c>
@@ -74036,7 +74051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>125</v>
       </c>
@@ -74069,7 +74084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>125</v>
       </c>
@@ -74102,7 +74117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>125</v>
       </c>
@@ -74135,7 +74150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>125</v>
       </c>
@@ -74168,7 +74183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>125</v>
       </c>
@@ -74201,7 +74216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>125</v>
       </c>
@@ -74234,7 +74249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>125</v>
       </c>
@@ -74267,7 +74282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>125</v>
       </c>
@@ -74300,7 +74315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>125</v>
       </c>
@@ -74333,7 +74348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>125</v>
       </c>
@@ -74366,7 +74381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>125</v>
       </c>
@@ -74399,7 +74414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>125</v>
       </c>
@@ -74433,7 +74448,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M47">
+  <autoFilter ref="A1:M47" xr:uid="{00000000-0009-0000-0000-000006000000}">
     <filterColumn colId="1">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -74446,28 +74461,28 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="C1:Q7"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2:Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.85546875" style="31"/>
-    <col min="4" max="4" width="53.140625" style="31" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="31" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="31"/>
-    <col min="7" max="10" width="8.140625" style="31" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="31" customWidth="1"/>
-    <col min="12" max="12" width="7.140625" style="31" customWidth="1"/>
-    <col min="13" max="16" width="10.85546875" style="31" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" style="31" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="31"/>
+    <col min="1" max="3" width="8.88671875" style="31"/>
+    <col min="4" max="4" width="53.109375" style="31" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" style="31" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="31"/>
+    <col min="7" max="10" width="8.109375" style="31" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" style="31" customWidth="1"/>
+    <col min="12" max="12" width="7.109375" style="31" customWidth="1"/>
+    <col min="13" max="16" width="10.88671875" style="31" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" style="31" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:17" s="34" customFormat="1" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:17" s="34" customFormat="1" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C1" s="35" t="s">
         <v>151</v>
       </c>
@@ -74518,7 +74533,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="3:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="91">
         <v>1</v>
       </c>
@@ -74568,7 +74583,7 @@
 81 - 100</v>
       </c>
     </row>
-    <row r="3" spans="3:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:17" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="91">
         <v>2</v>
       </c>
@@ -74595,7 +74610,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="3:17" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:17" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="91">
         <v>3</v>
       </c>
@@ -74640,7 +74655,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="3:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:17" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="91">
         <v>4</v>
       </c>
@@ -74682,7 +74697,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="3:17" ht="99.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:17" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="91">
         <v>6</v>
       </c>
@@ -74724,7 +74739,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="3:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:17" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="91">
         <v>7</v>
       </c>
@@ -74755,7 +74770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -74763,17 +74778,17 @@
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="78.140625" style="100" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="106" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="86.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="78.109375" style="100" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="106" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
+    <col min="5" max="5" width="86.5546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>597</v>
       </c>
@@ -74790,7 +74805,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>599</v>
       </c>
@@ -74805,7 +74820,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>600</v>
       </c>
@@ -74820,7 +74835,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>601</v>
       </c>
@@ -74835,7 +74850,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>602</v>
       </c>
@@ -74850,7 +74865,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>603</v>
       </c>
@@ -74865,7 +74880,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>604</v>
       </c>
@@ -74880,7 +74895,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>605</v>
       </c>
@@ -74895,7 +74910,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>606</v>
       </c>
@@ -74910,7 +74925,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>607</v>
       </c>
@@ -74922,7 +74937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>608</v>
       </c>
@@ -74934,7 +74949,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>609</v>
       </c>
@@ -74946,7 +74961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>589</v>
       </c>
@@ -74958,7 +74973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>590</v>
       </c>
@@ -74970,7 +74985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>591</v>
       </c>
@@ -74982,7 +74997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>610</v>
       </c>
@@ -74997,7 +75012,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>611</v>
       </c>
@@ -75012,7 +75027,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>612</v>
       </c>
@@ -75027,7 +75042,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>613</v>
       </c>
@@ -75042,7 +75057,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>614</v>
       </c>
@@ -75057,7 +75072,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>592</v>
       </c>
@@ -75069,7 +75084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>593</v>
       </c>
@@ -75081,7 +75096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>594</v>
       </c>
@@ -75093,7 +75108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>595</v>
       </c>
@@ -75105,7 +75120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>596</v>
       </c>
@@ -75117,69 +75132,69 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C26" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C27" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C28" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C29" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C30" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C31" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C32" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" s="106">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G35">
-    <sortState ref="A2:G35">
+  <autoFilter ref="A1:G35" xr:uid="{00000000-0009-0000-0000-000008000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G35">
       <sortCondition ref="B1:B35"/>
     </sortState>
   </autoFilter>

</xml_diff>